<commit_message>
Close to working version before removing old new cargo dist structure
</commit_message>
<xml_diff>
--- a/InputData/trans/ESF/ESF.xlsx
+++ b/InputData/trans/ESF/ESF.xlsx
@@ -1,23 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rorvis\Dropbox (Energy InNovation)\My Documents\Energy Policy Solutions\US\Models\eps-us\InputData\trans\ESF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC50FF20-7683-4757-ABD1-F239BFA39B59}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88AD7CC2-768E-426D-ADE5-986D83B820A0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AEO 2021 Table 39" sheetId="2" r:id="rId1"/>
     <sheet name="AEO 2021 Table 41" sheetId="3" r:id="rId2"/>
     <sheet name="AEO 2020 Table 39" sheetId="4" r:id="rId3"/>
     <sheet name="AEO 2020 Table 41" sheetId="5" r:id="rId4"/>
-    <sheet name="ESF" sheetId="1" r:id="rId5"/>
+    <sheet name="Sheet2" sheetId="7" r:id="rId5"/>
+    <sheet name="ESF" sheetId="1" r:id="rId6"/>
+    <sheet name="ESF (2)" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029" calcOnSave="0"/>
   <extLst>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="586" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="276">
   <si>
     <t>LDVs</t>
   </si>
@@ -6325,7 +6327,7 @@
   <dimension ref="A1:AK32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B71" sqref="A1:XFD1048576"/>
+      <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16404,10 +16406,24 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1810BF2B-0FB0-4CC7-90E9-8E246F7D37B2}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I33" sqref="I33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AF7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2:AF2"/>
     </sheetView>
   </sheetViews>
@@ -16513,128 +16529,857 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <f>1-('AEO 2021 Table 41'!F25*10^3/'AEO 2021 Table 39'!F50)/('AEO 2020 Table 41'!E25*10^3/'AEO 2020 Table 39'!E50)</f>
+        <f>(1-'AEO 2021 Table 41'!F26/'AEO 2021 Table 41'!$AJ$26)</f>
+        <v>9.6115567968204196E-2</v>
+      </c>
+      <c r="C2">
+        <f>(1-'AEO 2021 Table 41'!G26/'AEO 2021 Table 41'!$AJ$26)</f>
+        <v>4.830235589027887E-2</v>
+      </c>
+      <c r="D2">
+        <f>(1-'AEO 2021 Table 41'!H26/'AEO 2021 Table 41'!$AJ$26)</f>
+        <v>4.48005780273526E-2</v>
+      </c>
+      <c r="E2">
+        <f>(1-'AEO 2021 Table 41'!I26/'AEO 2021 Table 41'!$AJ$26)</f>
+        <v>3.770733953181904E-2</v>
+      </c>
+      <c r="F2">
+        <f>(1-'AEO 2021 Table 41'!J26/'AEO 2021 Table 41'!$AJ$26)</f>
+        <v>3.0230163489306849E-2</v>
+      </c>
+      <c r="G2">
+        <f>(1-'AEO 2021 Table 41'!K26/'AEO 2021 Table 41'!$AJ$26)</f>
+        <v>2.2991142462424508E-2</v>
+      </c>
+      <c r="H2">
+        <f>(1-'AEO 2021 Table 41'!L26/'AEO 2021 Table 41'!$AJ$26)</f>
+        <v>1.7090446571778051E-2</v>
+      </c>
+      <c r="I2">
+        <f>(1-'AEO 2021 Table 41'!M26/'AEO 2021 Table 41'!$AJ$26)</f>
+        <v>1.329064833111282E-2</v>
+      </c>
+      <c r="J2">
+        <f>(1-'AEO 2021 Table 41'!N26/'AEO 2021 Table 41'!$AJ$26)</f>
+        <v>9.709178067021984E-3</v>
+      </c>
+      <c r="K2">
+        <f>(1-'AEO 2021 Table 41'!O26/'AEO 2021 Table 41'!$AJ$26)</f>
+        <v>7.2569268412230326E-3</v>
+      </c>
+      <c r="L2">
+        <f>(1-'AEO 2021 Table 41'!P26/'AEO 2021 Table 41'!$AJ$26)</f>
+        <v>5.9519541660335573E-3</v>
+      </c>
+      <c r="M2">
+        <f>(1-'AEO 2021 Table 41'!Q26/'AEO 2021 Table 41'!$AJ$26)</f>
+        <v>6.2834038538076564E-3</v>
+      </c>
+      <c r="N2">
+        <f>(1-'AEO 2021 Table 41'!R26/'AEO 2021 Table 41'!$AJ$26)</f>
+        <v>7.5107590505245625E-3</v>
+      </c>
+      <c r="O2">
+        <f>(1-'AEO 2021 Table 41'!S26/'AEO 2021 Table 41'!$AJ$26)</f>
+        <v>8.1596719101499904E-3</v>
+      </c>
+      <c r="P2">
+        <f>(1-'AEO 2021 Table 41'!T26/'AEO 2021 Table 41'!$AJ$26)</f>
+        <v>8.7703908224477933E-3</v>
+      </c>
+      <c r="Q2">
+        <f>(1-'AEO 2021 Table 41'!U26/'AEO 2021 Table 41'!$AJ$26)</f>
+        <v>8.8516202033838143E-3</v>
+      </c>
+      <c r="R2">
+        <f>(1-'AEO 2021 Table 41'!V26/'AEO 2021 Table 41'!$AJ$26)</f>
+        <v>8.548220396443873E-3</v>
+      </c>
+      <c r="S2">
+        <f>(1-'AEO 2021 Table 41'!W26/'AEO 2021 Table 41'!$AJ$26)</f>
+        <v>8.3630911829387644E-3</v>
+      </c>
+      <c r="T2">
+        <f>(1-'AEO 2021 Table 41'!X26/'AEO 2021 Table 41'!$AJ$26)</f>
+        <v>8.2508916596023552E-3</v>
+      </c>
+      <c r="U2">
+        <f>(1-'AEO 2021 Table 41'!Y26/'AEO 2021 Table 41'!$AJ$26)</f>
+        <v>7.7875691074136277E-3</v>
+      </c>
+      <c r="V2">
+        <f>(1-'AEO 2021 Table 41'!Z26/'AEO 2021 Table 41'!$AJ$26)</f>
+        <v>7.149876200121863E-3</v>
+      </c>
+      <c r="W2">
+        <f>(1-'AEO 2021 Table 41'!AA26/'AEO 2021 Table 41'!$AJ$26)</f>
+        <v>6.3231347809069582E-3</v>
+      </c>
+      <c r="X2">
+        <f>(1-'AEO 2021 Table 41'!AB26/'AEO 2021 Table 41'!$AJ$26)</f>
+        <v>5.4097077025664353E-3</v>
+      </c>
+      <c r="Y2">
+        <f>(1-'AEO 2021 Table 41'!AC26/'AEO 2021 Table 41'!$AJ$26)</f>
+        <v>4.5187973778817447E-3</v>
+      </c>
+      <c r="Z2">
+        <f>(1-'AEO 2021 Table 41'!AD26/'AEO 2021 Table 41'!$AJ$26)</f>
+        <v>3.9073099756979923E-3</v>
+      </c>
+      <c r="AA2">
+        <f>(1-'AEO 2021 Table 41'!AE26/'AEO 2021 Table 41'!$AJ$26)</f>
+        <v>3.5784731535358771E-3</v>
+      </c>
+      <c r="AB2">
+        <f>(1-'AEO 2021 Table 41'!AF26/'AEO 2021 Table 41'!$AJ$26)</f>
+        <v>2.9993391755470666E-3</v>
+      </c>
+      <c r="AC2">
+        <f>(1-'AEO 2021 Table 41'!AG26/'AEO 2021 Table 41'!$AJ$26)</f>
+        <v>2.5364008683013139E-3</v>
+      </c>
+      <c r="AD2">
+        <f>(1-'AEO 2021 Table 41'!AH26/'AEO 2021 Table 41'!$AJ$26)</f>
+        <v>1.7451636818134331E-3</v>
+      </c>
+      <c r="AE2">
+        <f>(1-'AEO 2021 Table 41'!AI26/'AEO 2021 Table 41'!$AJ$26)</f>
+        <v>8.7054534270913919E-4</v>
+      </c>
+      <c r="AF2">
+        <f>(1-'AEO 2021 Table 41'!AJ26/'AEO 2021 Table 41'!$AJ$26)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <v>0</v>
+      </c>
+      <c r="R3">
+        <v>0</v>
+      </c>
+      <c r="S3">
+        <v>0</v>
+      </c>
+      <c r="T3">
+        <v>0</v>
+      </c>
+      <c r="U3">
+        <v>0</v>
+      </c>
+      <c r="V3">
+        <v>0</v>
+      </c>
+      <c r="W3">
+        <v>0</v>
+      </c>
+      <c r="X3">
+        <v>0</v>
+      </c>
+      <c r="Y3">
+        <v>0</v>
+      </c>
+      <c r="Z3">
+        <v>0</v>
+      </c>
+      <c r="AA3">
+        <v>0</v>
+      </c>
+      <c r="AB3">
+        <v>0</v>
+      </c>
+      <c r="AC3">
+        <v>0</v>
+      </c>
+      <c r="AD3">
+        <v>0</v>
+      </c>
+      <c r="AE3">
+        <v>0</v>
+      </c>
+      <c r="AF3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <v>0</v>
+      </c>
+      <c r="R4">
+        <v>0</v>
+      </c>
+      <c r="S4">
+        <v>0</v>
+      </c>
+      <c r="T4">
+        <v>0</v>
+      </c>
+      <c r="U4">
+        <v>0</v>
+      </c>
+      <c r="V4">
+        <v>0</v>
+      </c>
+      <c r="W4">
+        <v>0</v>
+      </c>
+      <c r="X4">
+        <v>0</v>
+      </c>
+      <c r="Y4">
+        <v>0</v>
+      </c>
+      <c r="Z4">
+        <v>0</v>
+      </c>
+      <c r="AA4">
+        <v>0</v>
+      </c>
+      <c r="AB4">
+        <v>0</v>
+      </c>
+      <c r="AC4">
+        <v>0</v>
+      </c>
+      <c r="AD4">
+        <v>0</v>
+      </c>
+      <c r="AE4">
+        <v>0</v>
+      </c>
+      <c r="AF4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <v>0</v>
+      </c>
+      <c r="R5">
+        <v>0</v>
+      </c>
+      <c r="S5">
+        <v>0</v>
+      </c>
+      <c r="T5">
+        <v>0</v>
+      </c>
+      <c r="U5">
+        <v>0</v>
+      </c>
+      <c r="V5">
+        <v>0</v>
+      </c>
+      <c r="W5">
+        <v>0</v>
+      </c>
+      <c r="X5">
+        <v>0</v>
+      </c>
+      <c r="Y5">
+        <v>0</v>
+      </c>
+      <c r="Z5">
+        <v>0</v>
+      </c>
+      <c r="AA5">
+        <v>0</v>
+      </c>
+      <c r="AB5">
+        <v>0</v>
+      </c>
+      <c r="AC5">
+        <v>0</v>
+      </c>
+      <c r="AD5">
+        <v>0</v>
+      </c>
+      <c r="AE5">
+        <v>0</v>
+      </c>
+      <c r="AF5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+      <c r="Q6">
+        <v>0</v>
+      </c>
+      <c r="R6">
+        <v>0</v>
+      </c>
+      <c r="S6">
+        <v>0</v>
+      </c>
+      <c r="T6">
+        <v>0</v>
+      </c>
+      <c r="U6">
+        <v>0</v>
+      </c>
+      <c r="V6">
+        <v>0</v>
+      </c>
+      <c r="W6">
+        <v>0</v>
+      </c>
+      <c r="X6">
+        <v>0</v>
+      </c>
+      <c r="Y6">
+        <v>0</v>
+      </c>
+      <c r="Z6">
+        <v>0</v>
+      </c>
+      <c r="AA6">
+        <v>0</v>
+      </c>
+      <c r="AB6">
+        <v>0</v>
+      </c>
+      <c r="AC6">
+        <v>0</v>
+      </c>
+      <c r="AD6">
+        <v>0</v>
+      </c>
+      <c r="AE6">
+        <v>0</v>
+      </c>
+      <c r="AF6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+      <c r="Q7">
+        <v>0</v>
+      </c>
+      <c r="R7">
+        <v>0</v>
+      </c>
+      <c r="S7">
+        <v>0</v>
+      </c>
+      <c r="T7">
+        <v>0</v>
+      </c>
+      <c r="U7">
+        <v>0</v>
+      </c>
+      <c r="V7">
+        <v>0</v>
+      </c>
+      <c r="W7">
+        <v>0</v>
+      </c>
+      <c r="X7">
+        <v>0</v>
+      </c>
+      <c r="Y7">
+        <v>0</v>
+      </c>
+      <c r="Z7">
+        <v>0</v>
+      </c>
+      <c r="AA7">
+        <v>0</v>
+      </c>
+      <c r="AB7">
+        <v>0</v>
+      </c>
+      <c r="AC7">
+        <v>0</v>
+      </c>
+      <c r="AD7">
+        <v>0</v>
+      </c>
+      <c r="AE7">
+        <v>0</v>
+      </c>
+      <c r="AF7">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE5205A5-4F6A-4D4A-924D-048B268B86A8}">
+  <dimension ref="A1:AF7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="B1">
+        <v>2020</v>
+      </c>
+      <c r="C1">
+        <v>2021</v>
+      </c>
+      <c r="D1">
+        <v>2022</v>
+      </c>
+      <c r="E1">
+        <v>2023</v>
+      </c>
+      <c r="F1">
+        <v>2024</v>
+      </c>
+      <c r="G1">
+        <v>2025</v>
+      </c>
+      <c r="H1">
+        <v>2026</v>
+      </c>
+      <c r="I1">
+        <v>2027</v>
+      </c>
+      <c r="J1">
+        <v>2028</v>
+      </c>
+      <c r="K1">
+        <v>2029</v>
+      </c>
+      <c r="L1">
+        <v>2030</v>
+      </c>
+      <c r="M1">
+        <v>2031</v>
+      </c>
+      <c r="N1">
+        <v>2032</v>
+      </c>
+      <c r="O1">
+        <v>2033</v>
+      </c>
+      <c r="P1">
+        <v>2034</v>
+      </c>
+      <c r="Q1">
+        <v>2035</v>
+      </c>
+      <c r="R1">
+        <v>2036</v>
+      </c>
+      <c r="S1">
+        <v>2037</v>
+      </c>
+      <c r="T1">
+        <v>2038</v>
+      </c>
+      <c r="U1">
+        <v>2039</v>
+      </c>
+      <c r="V1">
+        <v>2040</v>
+      </c>
+      <c r="W1">
+        <v>2041</v>
+      </c>
+      <c r="X1">
+        <v>2042</v>
+      </c>
+      <c r="Y1">
+        <v>2043</v>
+      </c>
+      <c r="Z1">
+        <v>2044</v>
+      </c>
+      <c r="AA1">
+        <v>2045</v>
+      </c>
+      <c r="AB1">
+        <v>2046</v>
+      </c>
+      <c r="AC1">
+        <v>2047</v>
+      </c>
+      <c r="AD1">
+        <v>2048</v>
+      </c>
+      <c r="AE1">
+        <v>2049</v>
+      </c>
+      <c r="AF1">
+        <v>2050</v>
+      </c>
+    </row>
+    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <f>MAX(0,1-('AEO 2021 Table 41'!F25*10^3/'AEO 2021 Table 39'!F50)/('AEO 2020 Table 41'!E25*10^3/'AEO 2020 Table 39'!E50))</f>
         <v>0.10044122631923624</v>
       </c>
       <c r="C2">
-        <f>1-('AEO 2021 Table 41'!G25*10^3/'AEO 2021 Table 39'!G50)/('AEO 2020 Table 41'!F25*10^3/'AEO 2020 Table 39'!F50)</f>
+        <f>MAX(0,1-('AEO 2021 Table 41'!G25*10^3/'AEO 2021 Table 39'!G50)/('AEO 2020 Table 41'!F25*10^3/'AEO 2020 Table 39'!F50))</f>
         <v>4.9325470097368207E-2</v>
       </c>
       <c r="D2">
-        <f>1-('AEO 2021 Table 41'!H25*10^3/'AEO 2021 Table 39'!H50)/('AEO 2020 Table 41'!G25*10^3/'AEO 2020 Table 39'!G50)</f>
+        <f>MAX(0,1-('AEO 2021 Table 41'!H25*10^3/'AEO 2021 Table 39'!H50)/('AEO 2020 Table 41'!G25*10^3/'AEO 2020 Table 39'!G50))</f>
         <v>4.0906456264438229E-2</v>
       </c>
       <c r="E2">
-        <f>1-('AEO 2021 Table 41'!I25*10^3/'AEO 2021 Table 39'!I50)/('AEO 2020 Table 41'!H25*10^3/'AEO 2020 Table 39'!H50)</f>
+        <f>MAX(0,1-('AEO 2021 Table 41'!I25*10^3/'AEO 2021 Table 39'!I50)/('AEO 2020 Table 41'!H25*10^3/'AEO 2020 Table 39'!H50))</f>
         <v>2.6663563889148922E-2</v>
       </c>
       <c r="F2">
-        <f>1-('AEO 2021 Table 41'!J25*10^3/'AEO 2021 Table 39'!J50)/('AEO 2020 Table 41'!I25*10^3/'AEO 2020 Table 39'!I50)</f>
+        <f>MAX(0,1-('AEO 2021 Table 41'!J25*10^3/'AEO 2021 Table 39'!J50)/('AEO 2020 Table 41'!I25*10^3/'AEO 2020 Table 39'!I50))</f>
         <v>1.1305739207200682E-2</v>
       </c>
       <c r="G2">
-        <f>1-('AEO 2021 Table 41'!K25*10^3/'AEO 2021 Table 39'!K50)/('AEO 2020 Table 41'!J25*10^3/'AEO 2020 Table 39'!J50)</f>
-        <v>-3.1189392549531014E-3</v>
+        <f>MAX(0,1-('AEO 2021 Table 41'!K25*10^3/'AEO 2021 Table 39'!K50)/('AEO 2020 Table 41'!J25*10^3/'AEO 2020 Table 39'!J50))</f>
+        <v>0</v>
       </c>
       <c r="H2">
-        <f>1-('AEO 2021 Table 41'!L25*10^3/'AEO 2021 Table 39'!L50)/('AEO 2020 Table 41'!K25*10^3/'AEO 2020 Table 39'!K50)</f>
-        <v>-1.5485237494659021E-2</v>
+        <f>MAX(0,1-('AEO 2021 Table 41'!L25*10^3/'AEO 2021 Table 39'!L50)/('AEO 2020 Table 41'!K25*10^3/'AEO 2020 Table 39'!K50))</f>
+        <v>0</v>
       </c>
       <c r="I2">
-        <f>1-('AEO 2021 Table 41'!M25*10^3/'AEO 2021 Table 39'!M50)/('AEO 2020 Table 41'!L25*10^3/'AEO 2020 Table 39'!L50)</f>
-        <v>-2.1938176469919135E-2</v>
+        <f>MAX(0,1-('AEO 2021 Table 41'!M25*10^3/'AEO 2021 Table 39'!M50)/('AEO 2020 Table 41'!L25*10^3/'AEO 2020 Table 39'!L50))</f>
+        <v>0</v>
       </c>
       <c r="J2">
-        <f>1-('AEO 2021 Table 41'!N25*10^3/'AEO 2021 Table 39'!N50)/('AEO 2020 Table 41'!M25*10^3/'AEO 2020 Table 39'!M50)</f>
-        <v>-2.6137878037502338E-2</v>
+        <f>MAX(0,1-('AEO 2021 Table 41'!N25*10^3/'AEO 2021 Table 39'!N50)/('AEO 2020 Table 41'!M25*10^3/'AEO 2020 Table 39'!M50))</f>
+        <v>0</v>
       </c>
       <c r="K2">
-        <f>1-('AEO 2021 Table 41'!O25*10^3/'AEO 2021 Table 39'!O50)/('AEO 2020 Table 41'!N25*10^3/'AEO 2020 Table 39'!N50)</f>
-        <v>-2.8120500438775453E-2</v>
+        <f>MAX(0,1-('AEO 2021 Table 41'!O25*10^3/'AEO 2021 Table 39'!O50)/('AEO 2020 Table 41'!N25*10^3/'AEO 2020 Table 39'!N50))</f>
+        <v>0</v>
       </c>
       <c r="L2">
-        <f>1-('AEO 2021 Table 41'!P25*10^3/'AEO 2021 Table 39'!P50)/('AEO 2020 Table 41'!O25*10^3/'AEO 2020 Table 39'!O50)</f>
-        <v>-2.9410349695861093E-2</v>
+        <f>MAX(0,1-('AEO 2021 Table 41'!P25*10^3/'AEO 2021 Table 39'!P50)/('AEO 2020 Table 41'!O25*10^3/'AEO 2020 Table 39'!O50))</f>
+        <v>0</v>
       </c>
       <c r="M2">
-        <f>1-('AEO 2021 Table 41'!Q25*10^3/'AEO 2021 Table 39'!Q50)/('AEO 2020 Table 41'!P25*10^3/'AEO 2020 Table 39'!P50)</f>
-        <v>-2.8356188977036734E-2</v>
+        <f>MAX(0,1-('AEO 2021 Table 41'!Q25*10^3/'AEO 2021 Table 39'!Q50)/('AEO 2020 Table 41'!P25*10^3/'AEO 2020 Table 39'!P50))</f>
+        <v>0</v>
       </c>
       <c r="N2">
-        <f>1-('AEO 2021 Table 41'!R25*10^3/'AEO 2021 Table 39'!R50)/('AEO 2020 Table 41'!Q25*10^3/'AEO 2020 Table 39'!Q50)</f>
-        <v>-2.631670005451614E-2</v>
+        <f>MAX(0,1-('AEO 2021 Table 41'!R25*10^3/'AEO 2021 Table 39'!R50)/('AEO 2020 Table 41'!Q25*10^3/'AEO 2020 Table 39'!Q50))</f>
+        <v>0</v>
       </c>
       <c r="O2">
-        <f>1-('AEO 2021 Table 41'!S25*10^3/'AEO 2021 Table 39'!S50)/('AEO 2020 Table 41'!R25*10^3/'AEO 2020 Table 39'!R50)</f>
-        <v>-2.5813230592213632E-2</v>
+        <f>MAX(0,1-('AEO 2021 Table 41'!S25*10^3/'AEO 2021 Table 39'!S50)/('AEO 2020 Table 41'!R25*10^3/'AEO 2020 Table 39'!R50))</f>
+        <v>0</v>
       </c>
       <c r="P2">
-        <f>1-('AEO 2021 Table 41'!T25*10^3/'AEO 2021 Table 39'!T50)/('AEO 2020 Table 41'!S25*10^3/'AEO 2020 Table 39'!S50)</f>
-        <v>-2.4998906852699454E-2</v>
+        <f>MAX(0,1-('AEO 2021 Table 41'!T25*10^3/'AEO 2021 Table 39'!T50)/('AEO 2020 Table 41'!S25*10^3/'AEO 2020 Table 39'!S50))</f>
+        <v>0</v>
       </c>
       <c r="Q2">
-        <f>1-('AEO 2021 Table 41'!U25*10^3/'AEO 2021 Table 39'!U50)/('AEO 2020 Table 41'!T25*10^3/'AEO 2020 Table 39'!T50)</f>
-        <v>-2.5450612674597695E-2</v>
+        <f>MAX(0,1-('AEO 2021 Table 41'!U25*10^3/'AEO 2021 Table 39'!U50)/('AEO 2020 Table 41'!T25*10^3/'AEO 2020 Table 39'!T50))</f>
+        <v>0</v>
       </c>
       <c r="R2">
-        <f>1-('AEO 2021 Table 41'!V25*10^3/'AEO 2021 Table 39'!V50)/('AEO 2020 Table 41'!U25*10^3/'AEO 2020 Table 39'!U50)</f>
-        <v>-2.6899861718024276E-2</v>
+        <f>MAX(0,1-('AEO 2021 Table 41'!V25*10^3/'AEO 2021 Table 39'!V50)/('AEO 2020 Table 41'!U25*10^3/'AEO 2020 Table 39'!U50))</f>
+        <v>0</v>
       </c>
       <c r="S2">
-        <f>1-('AEO 2021 Table 41'!W25*10^3/'AEO 2021 Table 39'!W50)/('AEO 2020 Table 41'!V25*10^3/'AEO 2020 Table 39'!V50)</f>
-        <v>-2.646790073620231E-2</v>
+        <f>MAX(0,1-('AEO 2021 Table 41'!W25*10^3/'AEO 2021 Table 39'!W50)/('AEO 2020 Table 41'!V25*10^3/'AEO 2020 Table 39'!V50))</f>
+        <v>0</v>
       </c>
       <c r="T2">
-        <f>1-('AEO 2021 Table 41'!X25*10^3/'AEO 2021 Table 39'!X50)/('AEO 2020 Table 41'!W25*10^3/'AEO 2020 Table 39'!W50)</f>
-        <v>-2.5696378026523359E-2</v>
+        <f>MAX(0,1-('AEO 2021 Table 41'!X25*10^3/'AEO 2021 Table 39'!X50)/('AEO 2020 Table 41'!W25*10^3/'AEO 2020 Table 39'!W50))</f>
+        <v>0</v>
       </c>
       <c r="U2">
-        <f>1-('AEO 2021 Table 41'!Y25*10^3/'AEO 2021 Table 39'!Y50)/('AEO 2020 Table 41'!X25*10^3/'AEO 2020 Table 39'!X50)</f>
-        <v>-2.5860399928624656E-2</v>
+        <f>MAX(0,1-('AEO 2021 Table 41'!Y25*10^3/'AEO 2021 Table 39'!Y50)/('AEO 2020 Table 41'!X25*10^3/'AEO 2020 Table 39'!X50))</f>
+        <v>0</v>
       </c>
       <c r="V2">
-        <f>1-('AEO 2021 Table 41'!Z25*10^3/'AEO 2021 Table 39'!Z50)/('AEO 2020 Table 41'!Y25*10^3/'AEO 2020 Table 39'!Y50)</f>
-        <v>-2.7062388377595559E-2</v>
+        <f>MAX(0,1-('AEO 2021 Table 41'!Z25*10^3/'AEO 2021 Table 39'!Z50)/('AEO 2020 Table 41'!Y25*10^3/'AEO 2020 Table 39'!Y50))</f>
+        <v>0</v>
       </c>
       <c r="W2">
-        <f>1-('AEO 2021 Table 41'!AA25*10^3/'AEO 2021 Table 39'!AA50)/('AEO 2020 Table 41'!Z25*10^3/'AEO 2020 Table 39'!Z50)</f>
-        <v>-2.767112059999377E-2</v>
+        <f>MAX(0,1-('AEO 2021 Table 41'!AA25*10^3/'AEO 2021 Table 39'!AA50)/('AEO 2020 Table 41'!Z25*10^3/'AEO 2020 Table 39'!Z50))</f>
+        <v>0</v>
       </c>
       <c r="X2">
-        <f>1-('AEO 2021 Table 41'!AB25*10^3/'AEO 2021 Table 39'!AB50)/('AEO 2020 Table 41'!AA25*10^3/'AEO 2020 Table 39'!AA50)</f>
-        <v>-2.9056941182366236E-2</v>
+        <f>MAX(0,1-('AEO 2021 Table 41'!AB25*10^3/'AEO 2021 Table 39'!AB50)/('AEO 2020 Table 41'!AA25*10^3/'AEO 2020 Table 39'!AA50))</f>
+        <v>0</v>
       </c>
       <c r="Y2">
-        <f>1-('AEO 2021 Table 41'!AC25*10^3/'AEO 2021 Table 39'!AC50)/('AEO 2020 Table 41'!AB25*10^3/'AEO 2020 Table 39'!AB50)</f>
-        <v>-3.0478291570334104E-2</v>
+        <f>MAX(0,1-('AEO 2021 Table 41'!AC25*10^3/'AEO 2021 Table 39'!AC50)/('AEO 2020 Table 41'!AB25*10^3/'AEO 2020 Table 39'!AB50))</f>
+        <v>0</v>
       </c>
       <c r="Z2">
-        <f>1-('AEO 2021 Table 41'!AD25*10^3/'AEO 2021 Table 39'!AD50)/('AEO 2020 Table 41'!AC25*10^3/'AEO 2020 Table 39'!AC50)</f>
-        <v>-3.114001296698321E-2</v>
+        <f>MAX(0,1-('AEO 2021 Table 41'!AD25*10^3/'AEO 2021 Table 39'!AD50)/('AEO 2020 Table 41'!AC25*10^3/'AEO 2020 Table 39'!AC50))</f>
+        <v>0</v>
       </c>
       <c r="AA2">
-        <f>1-('AEO 2021 Table 41'!AE25*10^3/'AEO 2021 Table 39'!AE50)/('AEO 2020 Table 41'!AD25*10^3/'AEO 2020 Table 39'!AD50)</f>
-        <v>-3.1403391695747906E-2</v>
+        <f>MAX(0,1-('AEO 2021 Table 41'!AE25*10^3/'AEO 2021 Table 39'!AE50)/('AEO 2020 Table 41'!AD25*10^3/'AEO 2020 Table 39'!AD50))</f>
+        <v>0</v>
       </c>
       <c r="AB2">
-        <f>1-('AEO 2021 Table 41'!AF25*10^3/'AEO 2021 Table 39'!AF50)/('AEO 2020 Table 41'!AE25*10^3/'AEO 2020 Table 39'!AE50)</f>
-        <v>-3.2405387677630015E-2</v>
+        <f>MAX(0,1-('AEO 2021 Table 41'!AF25*10^3/'AEO 2021 Table 39'!AF50)/('AEO 2020 Table 41'!AE25*10^3/'AEO 2020 Table 39'!AE50))</f>
+        <v>0</v>
       </c>
       <c r="AC2">
-        <f>1-('AEO 2021 Table 41'!AG25*10^3/'AEO 2021 Table 39'!AG50)/('AEO 2020 Table 41'!AF25*10^3/'AEO 2020 Table 39'!AF50)</f>
-        <v>-3.2733667172191394E-2</v>
+        <f>MAX(0,1-('AEO 2021 Table 41'!AG25*10^3/'AEO 2021 Table 39'!AG50)/('AEO 2020 Table 41'!AF25*10^3/'AEO 2020 Table 39'!AF50))</f>
+        <v>0</v>
       </c>
       <c r="AD2">
-        <f>1-('AEO 2021 Table 41'!AH25*10^3/'AEO 2021 Table 39'!AH50)/('AEO 2020 Table 41'!AG25*10^3/'AEO 2020 Table 39'!AG50)</f>
-        <v>-3.3038655102930914E-2</v>
+        <f>MAX(0,1-('AEO 2021 Table 41'!AH25*10^3/'AEO 2021 Table 39'!AH50)/('AEO 2020 Table 41'!AG25*10^3/'AEO 2020 Table 39'!AG50))</f>
+        <v>0</v>
       </c>
       <c r="AE2">
-        <f>1-('AEO 2021 Table 41'!AI25*10^3/'AEO 2021 Table 39'!AI50)/('AEO 2020 Table 41'!AH25*10^3/'AEO 2020 Table 39'!AH50)</f>
-        <v>-3.3640827972136078E-2</v>
+        <f>MAX(0,1-('AEO 2021 Table 41'!AI25*10^3/'AEO 2021 Table 39'!AI50)/('AEO 2020 Table 41'!AH25*10^3/'AEO 2020 Table 39'!AH50))</f>
+        <v>0</v>
       </c>
       <c r="AF2">
-        <f>1-('AEO 2021 Table 41'!AJ25*10^3/'AEO 2021 Table 39'!AJ50)/('AEO 2020 Table 41'!AI25*10^3/'AEO 2020 Table 39'!AI50)</f>
-        <v>-3.4350202987748713E-2</v>
+        <f>MAX(0,1-('AEO 2021 Table 41'!AJ25*10^3/'AEO 2021 Table 39'!AJ50)/('AEO 2020 Table 41'!AI25*10^3/'AEO 2020 Table 39'!AI50))</f>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.25">

</xml_diff>